<commit_message>
Reduce the number of JLCPCB's extended parts
</commit_message>
<xml_diff>
--- a/C64-Composite-Modulator-Bom.xlsx
+++ b/C64-Composite-Modulator-Bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KiCad\Projets\C64-Composite-Modulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B23E40-2E46-4E0E-876D-FC57EA90A9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5D30D1-7F53-4B4C-9183-3F157F0E3248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{734A0269-BCB0-4A9B-BB67-1ED98D9F55F5}"/>
+    <workbookView xWindow="6440" yWindow="4050" windowWidth="28800" windowHeight="15370" xr2:uid="{734A0269-BCB0-4A9B-BB67-1ED98D9F55F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
   <si>
     <t>Ref</t>
   </si>
@@ -117,15 +117,6 @@
     <t>Capacitor_SMD:C_0805_2012Metric</t>
   </si>
   <si>
-    <t>https://datasheet.lcsc.com/lcsc/1810241123_Samsung-Electro-Mechanics-CL21B333KBANNNC_C159777.pdf</t>
-  </si>
-  <si>
-    <t>CL21B333KBANNNC</t>
-  </si>
-  <si>
-    <t>C159777</t>
-  </si>
-  <si>
     <t>1276-1796-1-ND</t>
   </si>
   <si>
@@ -264,18 +255,9 @@
     <t>Inductor_SMD:L_0805_2012Metric</t>
   </si>
   <si>
-    <t>https://datasheet.lcsc.com/lcsc/2110081230_Sunlord-MCL2012H100MT_C95978.pdf</t>
-  </si>
-  <si>
     <t>Sunlord</t>
   </si>
   <si>
-    <t>MCL2012H100MT</t>
-  </si>
-  <si>
-    <t>C95978</t>
-  </si>
-  <si>
     <t>587-2452-1-ND</t>
   </si>
   <si>
@@ -532,6 +514,27 @@
   </si>
   <si>
     <t>CUI_Devices:RCJ-014</t>
+  </si>
+  <si>
+    <t>C1739</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1811061723_FH-Guangdong-Fenghua-Advanced-Tech-0805B333K500NT_C1739.pdf</t>
+  </si>
+  <si>
+    <t>FH(Guangdong Fenghua Advanced Tech)</t>
+  </si>
+  <si>
+    <t>0805B333K500NT</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2110081230_Sunlord-SDFL2012S100KTF_C1046.pdf</t>
+  </si>
+  <si>
+    <t>SDFL2012S100KTF</t>
+  </si>
+  <si>
+    <t>C1046</t>
   </si>
 </sst>
 </file>
@@ -587,12 +590,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C81D85E-0185-4F98-8DEF-805A20BC681E}" name="Tableau3" displayName="Tableau3" ref="A1:I30" totalsRowShown="0">
-  <autoFilter ref="A1:I30" xr:uid="{2C81D85E-0185-4F98-8DEF-805A20BC681E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I30">
-    <sortCondition ref="A2:A30"/>
-    <sortCondition ref="B2:B30"/>
-    <sortCondition ref="C2:C30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C81D85E-0185-4F98-8DEF-805A20BC681E}" name="Tableau3" displayName="Tableau3" ref="A1:I31" totalsRowShown="0">
+  <autoFilter ref="A1:I31" xr:uid="{2C81D85E-0185-4F98-8DEF-805A20BC681E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I20">
+    <sortCondition ref="A2:A20"/>
+    <sortCondition ref="B2:B20"/>
+    <sortCondition ref="C2:C20"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{64445715-8B21-4906-9AC8-CFA32B869934}" name="Ref"/>
@@ -1014,50 +1017,50 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" t="s">
         <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1083,614 +1086,614 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>56</v>
       </c>
-      <c r="F9" t="s">
+      <c r="I9" t="s">
         <v>57</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>62</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
         <v>63</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" t="s">
         <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
         <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
         <v>81</v>
       </c>
-      <c r="B14" t="s">
+      <c r="H14" t="s">
         <v>82</v>
-      </c>
-      <c r="C14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" t="s">
         <v>82</v>
-      </c>
-      <c r="C15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" t="s">
         <v>90</v>
       </c>
-      <c r="B16" t="s">
+      <c r="H16" t="s">
         <v>91</v>
-      </c>
-      <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H16" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G20" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G21" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="G22" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="H22" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" t="s">
         <v>128</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G26" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H26" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" t="s">
+        <v>139</v>
+      </c>
+      <c r="E27" t="s">
+        <v>140</v>
+      </c>
+      <c r="F27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" t="s">
         <v>143</v>
-      </c>
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" t="s">
-        <v>146</v>
-      </c>
-      <c r="F27" t="s">
-        <v>147</v>
-      </c>
-      <c r="G27" t="s">
-        <v>148</v>
-      </c>
-      <c r="H27" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" t="s">
         <v>150</v>
-      </c>
-      <c r="B28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C28" t="s">
-        <v>144</v>
-      </c>
-      <c r="D28" t="s">
-        <v>152</v>
-      </c>
-      <c r="E28" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H28" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" t="s">
+        <v>152</v>
+      </c>
+      <c r="G29" t="s">
+        <v>156</v>
+      </c>
+      <c r="H29" t="s">
         <v>157</v>
-      </c>
-      <c r="B29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" t="s">
-        <v>159</v>
-      </c>
-      <c r="D29" t="s">
-        <v>160</v>
-      </c>
-      <c r="E29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" t="s">
-        <v>158</v>
-      </c>
-      <c r="G29" t="s">
-        <v>162</v>
-      </c>
-      <c r="H29" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>

</xml_diff>